<commit_message>
Minor correction.[ja & en]
Minor correction.[ja & en]
</commit_message>
<xml_diff>
--- a/Pin/Spresense_pin_function_en.xlsx
+++ b/Pin/Spresense_pin_function_en.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0AD070-E8E1-4117-AE2A-66AC8E18AD38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D53ADF2-1933-45F7-8D34-B4DEC79A474D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D4A1A96D-02BA-4FB2-8190-975445C70E49}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pin List" sheetId="1" r:id="rId1"/>
+    <sheet name="Public history" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$AB$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pin List'!$A$2:$AB$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4097" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4103" uniqueCount="565">
   <si>
     <t>I/O</t>
   </si>
@@ -2031,6 +2032,35 @@
   </si>
   <si>
     <t>Low</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Low</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2020.11.13</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2021.4.14</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Contents</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>First draft.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Corrected the initial value of ACP_GPO1 to 7 after starting Arduino and SDK.
+Corrected each initial value of XRST (SPR_RST_X).</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2213,7 +2243,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2265,18 +2295,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2287,6 +2305,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2327,6 +2351,24 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2656,7 +2698,7 @@
   <dimension ref="A1:AB196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
@@ -2690,68 +2732,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="23" t="s">
         <v>526</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="21" t="s">
         <v>531</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="28" t="s">
         <v>529</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>530</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="26" t="s">
         <v>532</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="21" t="s">
         <v>527</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="21" t="s">
         <v>443</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="21" t="s">
         <v>528</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="32" t="s">
         <v>533</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="36" t="s">
+      <c r="N1" s="33"/>
+      <c r="O1" s="34" t="s">
         <v>536</v>
       </c>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="17" t="s">
+      <c r="P1" s="35"/>
+      <c r="Q1" s="36" t="s">
         <v>537</v>
       </c>
-      <c r="R1" s="18"/>
-      <c r="S1" s="19" t="s">
+      <c r="R1" s="37"/>
+      <c r="S1" s="21" t="s">
         <v>538</v>
       </c>
-      <c r="T1" s="32" t="s">
+      <c r="T1" s="30" t="s">
         <v>539</v>
       </c>
-      <c r="U1" s="33"/>
-      <c r="V1" s="24" t="s">
+      <c r="U1" s="31"/>
+      <c r="V1" s="20" t="s">
         <v>546</v>
       </c>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="21" t="s">
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="17" t="s">
         <v>547</v>
       </c>
-      <c r="AA1" s="23" t="s">
+      <c r="AA1" s="19" t="s">
         <v>548</v>
       </c>
-      <c r="AB1" s="24" t="s">
+      <c r="AB1" s="20" t="s">
         <v>549</v>
       </c>
     </row>
@@ -2768,14 +2810,14 @@
       <c r="D2" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
       <c r="M2" s="3" t="s">
         <v>443</v>
       </c>
@@ -2794,7 +2836,7 @@
       <c r="R2" s="15" t="s">
         <v>535</v>
       </c>
-      <c r="S2" s="20"/>
+      <c r="S2" s="22"/>
       <c r="T2" s="5" t="s">
         <v>540</v>
       </c>
@@ -2813,9 +2855,9 @@
       <c r="Y2" s="5" t="s">
         <v>545</v>
       </c>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="24"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
@@ -3832,19 +3874,19 @@
         <v>19</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>45</v>
+        <v>558</v>
       </c>
       <c r="O16" s="7" t="s">
         <v>41</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q16" s="7" t="s">
         <v>41</v>
       </c>
       <c r="R16" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S16" s="7" t="s">
         <v>43</v>
@@ -11526,19 +11568,19 @@
         <v>19</v>
       </c>
       <c r="N114" s="7" t="s">
-        <v>45</v>
+        <v>558</v>
       </c>
       <c r="O114" s="7" t="s">
         <v>41</v>
       </c>
       <c r="P114" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q114" s="7" t="s">
         <v>41</v>
       </c>
       <c r="R114" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S114" s="7" t="s">
         <v>43</v>
@@ -17883,6 +17925,11 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A2:AB2" xr:uid="{63397F36-E61B-4D89-81D6-261292303536}"/>
   <mergeCells count="18">
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="V1:Y1"/>
     <mergeCell ref="L1:L2"/>
@@ -17896,14 +17943,54 @@
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FF7299-453B-49A3-B9C8-70D3E9918ACE}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="50.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="38" t="s">
+        <v>561</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="39" t="s">
+        <v>559</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="39" t="s">
+        <v>560</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>564</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>